<commit_message>
HEADING TITLE UPDATED  for Live Casino
</commit_message>
<xml_diff>
--- a/Template/src/reports/HEADING TITLE CONTENT - CASINO LOBBY/HEADING TITLE CONTENT - CASINO LOBBY [TEMP].xlsx
+++ b/Template/src/reports/HEADING TITLE CONTENT - CASINO LOBBY/HEADING TITLE CONTENT - CASINO LOBBY [TEMP].xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="414" uniqueCount="95">
   <si>
     <t>Result of HEADING TITLE CONTENT - CASINO LOBBY</t>
   </si>
@@ -22,7 +22,7 @@
     <t>Start</t>
   </si>
   <si>
-    <t>2021-03-26 17:28:12</t>
+    <t>2021-03-29 00:15:49</t>
   </si>
   <si>
     <t>#</t>
@@ -55,91 +55,250 @@
     <t>-</t>
   </si>
   <si>
-    <t>Online Live Casino</t>
-  </si>
-  <si>
     <t>Live Casino Online</t>
   </si>
   <si>
+    <t>PASSED</t>
+  </si>
+  <si>
+    <t>Case chỉ có nhà cung cấp</t>
+  </si>
+  <si>
+    <t>All</t>
+  </si>
+  <si>
+    <t>Top 10 Trò Chơi Của Live Casino</t>
+  </si>
+  <si>
     <t>FAILED</t>
   </si>
   <si>
-    <t>Sắp xếp theo</t>
-  </si>
-  <si>
-    <t>None</t>
+    <t>Evolution</t>
+  </si>
+  <si>
+    <t>Top 7 Trò Chơi Của Evolution</t>
+  </si>
+  <si>
+    <t>Ebet</t>
+  </si>
+  <si>
+    <t>Top 6 Trò Chơi Của Ebet</t>
+  </si>
+  <si>
+    <t>VivoGaming</t>
+  </si>
+  <si>
+    <t>Top 3 Trò Chơi Của VivoGaming</t>
+  </si>
+  <si>
+    <t>Vivogaming</t>
+  </si>
+  <si>
+    <t>Allbet</t>
+  </si>
+  <si>
+    <t>Top 7 Trò Chơi Của Allbet</t>
+  </si>
+  <si>
+    <t>HGaming</t>
+  </si>
+  <si>
+    <t>Top 3 Trò Chơi Của HGaming</t>
+  </si>
+  <si>
+    <t>HoGaming</t>
   </si>
   <si>
     <t>Nhiều Người Chơi</t>
   </si>
   <si>
-    <t>Top 10 Trò Chơi Nhiều Người Chơi</t>
+    <t>Top 10 Trò Chơi Nhiều Người Chơi Của Live Casino</t>
   </si>
   <si>
     <t>Top 10 Trò Chơi Nhiều Người Chơi Của Live Casino Online</t>
   </si>
   <si>
+    <t>Baccarat</t>
+  </si>
+  <si>
+    <t>Top Baccarat Nhiều Người Chơi Live Casino</t>
+  </si>
+  <si>
+    <t>Top 1 Trò Chơi Baccarat Nhiều Người Chơi Của Live Casino Online</t>
+  </si>
+  <si>
+    <t>Roulette</t>
+  </si>
+  <si>
+    <t>Top 3 Trò Chơi Baccarat, Roulette Nhiều Người Chơi Live Casino</t>
+  </si>
+  <si>
+    <t>Top 3 Trò Chơi Baccarat, Roulette Nhiều Người Chơi Của Live Casino Online</t>
+  </si>
+  <si>
+    <t>Top Baccarat, Roulette Nhiều Người Chơi Live Casino</t>
+  </si>
+  <si>
+    <t>Top 10 Trò Chơi Baccarat Nhiều Người Chơi Live Casino</t>
+  </si>
+  <si>
+    <t>Top 2 Trò Chơi Roulette, Baccarat Live Casino</t>
+  </si>
+  <si>
+    <t>Top 2 Trò Chơi Roulette Nhiều Người Chơi Của Live Casino Online</t>
+  </si>
+  <si>
+    <t>Top 3 Trò Chơi Roulette, Baccarat Live Casino</t>
+  </si>
+  <si>
+    <t>Top 3 Trò Chơi Roulette, Baccarat Nhiều Người Chơi Của Live Casino Online</t>
+  </si>
+  <si>
+    <t>Top 10 Trò Chơi Roulette Live Casino</t>
+  </si>
+  <si>
     <t>Đang Hot</t>
   </si>
   <si>
-    <t>Top 10 Trò Chơi Đang Hot</t>
+    <t>Top 10 Trò Chơi Roulette Đang Hot Live Casino</t>
   </si>
   <si>
     <t>Top 10 Trò Chơi Đang Hot Của Live Casino Online</t>
   </si>
   <si>
+    <t>Top Baccarat, Roulette Đang Hot</t>
+  </si>
+  <si>
+    <t>Top 1 Trò Chơi Baccarat Đang Hot Của Live Casino Online</t>
+  </si>
+  <si>
+    <t>Top 3 Trò Chơi Baccarat, Roulette Đang Hot</t>
+  </si>
+  <si>
+    <t>Top 3 Trò Chơi Baccarat, Roulette Đang Hot Của Live Casino Online</t>
+  </si>
+  <si>
+    <t>Top 10 Trò Chơi Baccarat Đang Hot</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Baccarat, Roulette Online</t>
+  </si>
+  <si>
+    <t>Top 2 Trò Chơi Roulette Đang Hot Của Live Casino Online</t>
+  </si>
+  <si>
+    <t>Top 3 Trò Chơi Roulette, Baccarat Đang Hot Của Live Casino Online</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Roulette Online</t>
+  </si>
+  <si>
     <t>Phổ Biến</t>
   </si>
   <si>
-    <t>Top 10 Trò Chơi Phổ Biến</t>
+    <t>Top 10 Trò Chơi Roulette Phổ Biến</t>
   </si>
   <si>
     <t>Top 10 Trò Chơi Phổ Biến Của Live Casino Online</t>
   </si>
   <si>
+    <t>Top Baccarat Phổ Biến</t>
+  </si>
+  <si>
+    <t>Top 1 Trò Chơi Baccarat Phổ Biến Của Live Casino Online</t>
+  </si>
+  <si>
+    <t>Top 3 Trò Chơi Roulette, Baccarat Phổ Biến</t>
+  </si>
+  <si>
+    <t>Top 3 Trò Chơi Baccarat, Roulette Phổ Biến Của Live Casino Online</t>
+  </si>
+  <si>
+    <t>Top Roulette, Baccarat Phổ Biến</t>
+  </si>
+  <si>
+    <t>Top 10 Trò Chơi Baccarat Phổ Biến</t>
+  </si>
+  <si>
+    <t>Top 2 Trò Chơi Roulette Phổ Biến</t>
+  </si>
+  <si>
+    <t>Top 2 Trò Chơi Roulette Phổ Biến Của Live Casino Online</t>
+  </si>
+  <si>
+    <t>Top 3 Trò Chơi Baccarat, Roulette Phổ Biến</t>
+  </si>
+  <si>
+    <t>Top 3 Trò Chơi Roulette, Baccarat Phổ Biến Của Live Casino Online</t>
+  </si>
+  <si>
+    <t>Top 2 Trò Chơi Baccarat, Roulette Phổ Biến</t>
+  </si>
+  <si>
     <t>Mới Nhất</t>
   </si>
   <si>
-    <t>Top 10 Trò Chơi Mới Nhất</t>
+    <t>Top 10 Trò Chơi Roulette Mới Nhất</t>
   </si>
   <si>
     <t>Top 10 Trò Chơi Mới Nhất Của Live Casino Online</t>
   </si>
   <si>
-    <t>All</t>
-  </si>
-  <si>
-    <t>Top 10 Trò Chơi Nhiều Người Chơi Live Casino</t>
-  </si>
-  <si>
-    <t>Baccarat</t>
-  </si>
-  <si>
-    <t>Top Baccarat Nhiều Người Chơi Live Casino</t>
-  </si>
-  <si>
-    <t>Top 1 Trò Chơi Baccarat Của Live Casino Online</t>
-  </si>
-  <si>
-    <t>Roulette</t>
-  </si>
-  <si>
-    <t>Top 3 Trò Chơi Baccarat, Roulette Nhiều Người Chơi Live Casino</t>
-  </si>
-  <si>
-    <t>Top 3 Trò Chơi Baccarat, Roulette Của Live Casino Online</t>
-  </si>
-  <si>
-    <t>Top 2 Trò Chơi Roulette Nhiều Người Chơi Live Casino</t>
-  </si>
-  <si>
-    <t>Top 2 Trò Chơi Roulette Của Live Casino Online</t>
-  </si>
-  <si>
-    <t>Top 3 Trò Chơi Roulette, Baccarat Nhiều Người Chơi Live Casino</t>
-  </si>
-  <si>
-    <t>Top 3 Trò Chơi Roulette, Baccarat Của Live Casino Online</t>
+    <t>Top Baccarat Mới Nhất</t>
+  </si>
+  <si>
+    <t>Top 1 Trò Chơi Baccarat Mới Nhất Của Live Casino Online</t>
+  </si>
+  <si>
+    <t>Top 3 Trò Chơi Roulette, Baccarat Mới Nhất</t>
+  </si>
+  <si>
+    <t>Top 3 Trò Chơi Baccarat, Roulette Mới Nhất Của Live Casino Online</t>
+  </si>
+  <si>
+    <t>Top Roulette, Baccarat Mới Nhất</t>
+  </si>
+  <si>
+    <t>Top 10 Trò Chơi Baccarat Mới Nhất</t>
+  </si>
+  <si>
+    <t>Top 2 Trò Chơi Roulette Mới Nhất</t>
+  </si>
+  <si>
+    <t>Top 2 Trò Chơi Roulette Mới Nhất Của Live Casino Online</t>
+  </si>
+  <si>
+    <t>Top 3 Trò Chơi Baccarat, Roulette Mới Nhất</t>
+  </si>
+  <si>
+    <t>Top 3 Trò Chơi Roulette, Baccarat Mới Nhất Của Live Casino Online</t>
+  </si>
+  <si>
+    <t>Top 2 Trò Chơi Baccarat, Roulette Mới Nhất</t>
+  </si>
+  <si>
+    <t>Top 7 Trò Chơi Roulette Mới Nhất Của Evolution</t>
+  </si>
+  <si>
+    <t>Top 7 Trò Chơi Roulette Nhiều Người Chơi Của Evolution</t>
+  </si>
+  <si>
+    <t>Top 7 Trò Chơi Nhiều Người Chơi Của Evolution</t>
+  </si>
+  <si>
+    <t>Top Baccarat Nhiều Người Chơi Của Evolution</t>
+  </si>
+  <si>
+    <t>Top Trò Chơi Baccarat Nhiều Người Chơi Của Evolution</t>
+  </si>
+  <si>
+    <t>Top Roulette, Baccarat Nhiều Người Chơi Của Evolution</t>
+  </si>
+  <si>
+    <t>Top Trò Chơi Baccarat, Roulette Nhiều Người Chơi Của Evolution</t>
+  </si>
+  <si>
+    <t>Top 7 Trò Chơi Baccarat Nhiều Người Chơi Của Evolution</t>
   </si>
 </sst>
 </file>
@@ -176,7 +335,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -197,13 +356,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
+        <fgColor rgb="FF008000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF78ECF5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -227,12 +392,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -527,7 +693,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I20"/>
+  <dimension ref="A1:I55"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -598,10 +764,10 @@
         <v>13</v>
       </c>
       <c r="H5" t="s">
+        <v>13</v>
+      </c>
+      <c r="I5" s="3" t="s">
         <v>14</v>
-      </c>
-      <c r="I5" s="3" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="6" spans="1:9">
@@ -609,20 +775,12 @@
         <v>12</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="E6" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="F6" s="4" t="s">
-        <v>17</v>
-      </c>
+        <v>15</v>
+      </c>
+      <c r="C6" s="4"/>
+      <c r="D6" s="4"/>
+      <c r="E6" s="4"/>
+      <c r="F6" s="4"/>
       <c r="G6" s="4"/>
       <c r="H6" s="4"/>
       <c r="I6" s="4"/>
@@ -632,7 +790,7 @@
         <v>2</v>
       </c>
       <c r="B7" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C7" t="s">
         <v>12</v>
@@ -647,13 +805,13 @@
         <v>12</v>
       </c>
       <c r="G7" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="H7" t="s">
-        <v>20</v>
-      </c>
-      <c r="I7" s="3" t="s">
-        <v>15</v>
+        <v>13</v>
+      </c>
+      <c r="I7" s="5" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="8" spans="1:9">
@@ -661,7 +819,7 @@
         <v>3</v>
       </c>
       <c r="B8" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C8" t="s">
         <v>12</v>
@@ -676,13 +834,13 @@
         <v>12</v>
       </c>
       <c r="G8" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="H8" t="s">
-        <v>23</v>
-      </c>
-      <c r="I8" s="3" t="s">
-        <v>15</v>
+        <v>19</v>
+      </c>
+      <c r="I8" s="5" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="9" spans="1:9">
@@ -690,7 +848,7 @@
         <v>4</v>
       </c>
       <c r="B9" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C9" t="s">
         <v>12</v>
@@ -705,13 +863,13 @@
         <v>12</v>
       </c>
       <c r="G9" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="H9" t="s">
-        <v>26</v>
-      </c>
-      <c r="I9" s="3" t="s">
-        <v>15</v>
+        <v>21</v>
+      </c>
+      <c r="I9" s="5" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="10" spans="1:9">
@@ -719,7 +877,7 @@
         <v>5</v>
       </c>
       <c r="B10" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="C10" t="s">
         <v>12</v>
@@ -734,13 +892,13 @@
         <v>12</v>
       </c>
       <c r="G10" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="H10" t="s">
-        <v>29</v>
-      </c>
-      <c r="I10" s="3" t="s">
-        <v>15</v>
+        <v>25</v>
+      </c>
+      <c r="I10" s="5" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="11" spans="1:9">
@@ -748,10 +906,10 @@
         <v>6</v>
       </c>
       <c r="B11" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C11" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="D11" t="s">
         <v>12</v>
@@ -763,13 +921,13 @@
         <v>12</v>
       </c>
       <c r="G11" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="H11" t="s">
-        <v>20</v>
-      </c>
-      <c r="I11" s="3" t="s">
-        <v>15</v>
+        <v>26</v>
+      </c>
+      <c r="I11" s="5" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="12" spans="1:9">
@@ -777,28 +935,28 @@
         <v>7</v>
       </c>
       <c r="B12" t="s">
+        <v>28</v>
+      </c>
+      <c r="C12" t="s">
+        <v>12</v>
+      </c>
+      <c r="D12" t="s">
+        <v>12</v>
+      </c>
+      <c r="E12" t="s">
+        <v>12</v>
+      </c>
+      <c r="F12" t="s">
+        <v>12</v>
+      </c>
+      <c r="G12" t="s">
+        <v>29</v>
+      </c>
+      <c r="H12" t="s">
         <v>30</v>
       </c>
-      <c r="C12" t="s">
-        <v>18</v>
-      </c>
-      <c r="D12" t="s">
-        <v>12</v>
-      </c>
-      <c r="E12" t="s">
-        <v>12</v>
-      </c>
-      <c r="F12" t="s">
-        <v>12</v>
-      </c>
-      <c r="G12" t="s">
-        <v>31</v>
-      </c>
-      <c r="H12" t="s">
-        <v>14</v>
-      </c>
-      <c r="I12" s="3" t="s">
-        <v>15</v>
+      <c r="I12" s="5" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="13" spans="1:9">
@@ -806,13 +964,13 @@
         <v>8</v>
       </c>
       <c r="B13" t="s">
-        <v>32</v>
+        <v>16</v>
       </c>
       <c r="C13" t="s">
-        <v>30</v>
+        <v>12</v>
       </c>
       <c r="D13" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="E13" t="s">
         <v>12</v>
@@ -821,13 +979,13 @@
         <v>12</v>
       </c>
       <c r="G13" t="s">
-        <v>33</v>
+        <v>17</v>
       </c>
       <c r="H13" t="s">
-        <v>34</v>
-      </c>
-      <c r="I13" s="3" t="s">
-        <v>15</v>
+        <v>13</v>
+      </c>
+      <c r="I13" s="5" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="14" spans="1:9">
@@ -835,28 +993,28 @@
         <v>9</v>
       </c>
       <c r="B14" t="s">
+        <v>16</v>
+      </c>
+      <c r="C14" t="s">
+        <v>31</v>
+      </c>
+      <c r="D14" t="s">
+        <v>12</v>
+      </c>
+      <c r="E14" t="s">
+        <v>12</v>
+      </c>
+      <c r="F14" t="s">
+        <v>12</v>
+      </c>
+      <c r="G14" t="s">
         <v>32</v>
       </c>
-      <c r="C14" t="s">
-        <v>35</v>
-      </c>
-      <c r="D14" t="s">
-        <v>30</v>
-      </c>
-      <c r="E14" t="s">
-        <v>18</v>
-      </c>
-      <c r="F14" t="s">
-        <v>12</v>
-      </c>
-      <c r="G14" t="s">
-        <v>36</v>
-      </c>
       <c r="H14" t="s">
-        <v>37</v>
-      </c>
-      <c r="I14" s="3" t="s">
-        <v>15</v>
+        <v>33</v>
+      </c>
+      <c r="I14" s="5" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="15" spans="1:9">
@@ -864,13 +1022,13 @@
         <v>10</v>
       </c>
       <c r="B15" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C15" t="s">
-        <v>30</v>
+        <v>16</v>
       </c>
       <c r="D15" t="s">
-        <v>18</v>
+        <v>31</v>
       </c>
       <c r="E15" t="s">
         <v>12</v>
@@ -879,13 +1037,13 @@
         <v>12</v>
       </c>
       <c r="G15" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="H15" t="s">
-        <v>34</v>
-      </c>
-      <c r="I15" s="3" t="s">
-        <v>15</v>
+        <v>36</v>
+      </c>
+      <c r="I15" s="5" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="16" spans="1:9">
@@ -893,28 +1051,28 @@
         <v>11</v>
       </c>
       <c r="B16" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="C16" t="s">
-        <v>18</v>
+        <v>37</v>
       </c>
       <c r="D16" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="E16" t="s">
-        <v>12</v>
+        <v>31</v>
       </c>
       <c r="F16" t="s">
         <v>12</v>
       </c>
       <c r="G16" t="s">
-        <v>31</v>
+        <v>38</v>
       </c>
       <c r="H16" t="s">
-        <v>14</v>
-      </c>
-      <c r="I16" s="3" t="s">
-        <v>15</v>
+        <v>39</v>
+      </c>
+      <c r="I16" s="5" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="17" spans="1:9">
@@ -922,28 +1080,28 @@
         <v>12</v>
       </c>
       <c r="B17" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C17" t="s">
-        <v>30</v>
+        <v>37</v>
       </c>
       <c r="D17" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E17" t="s">
-        <v>12</v>
+        <v>31</v>
       </c>
       <c r="F17" t="s">
         <v>12</v>
       </c>
       <c r="G17" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="H17" t="s">
-        <v>39</v>
-      </c>
-      <c r="I17" s="3" t="s">
-        <v>15</v>
+        <v>36</v>
+      </c>
+      <c r="I17" s="5" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="18" spans="1:9">
@@ -951,28 +1109,28 @@
         <v>13</v>
       </c>
       <c r="B18" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C18" t="s">
-        <v>32</v>
+        <v>16</v>
       </c>
       <c r="D18" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="E18" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="F18" t="s">
         <v>12</v>
       </c>
       <c r="G18" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="H18" t="s">
-        <v>41</v>
-      </c>
-      <c r="I18" s="3" t="s">
-        <v>15</v>
+        <v>33</v>
+      </c>
+      <c r="I18" s="5" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="19" spans="1:9">
@@ -980,13 +1138,13 @@
         <v>14</v>
       </c>
       <c r="B19" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="C19" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="D19" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E19" t="s">
         <v>12</v>
@@ -995,13 +1153,13 @@
         <v>12</v>
       </c>
       <c r="G19" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="H19" t="s">
-        <v>39</v>
-      </c>
-      <c r="I19" s="3" t="s">
-        <v>15</v>
+        <v>43</v>
+      </c>
+      <c r="I19" s="5" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="20" spans="1:9">
@@ -1009,28 +1167,1043 @@
         <v>15</v>
       </c>
       <c r="B20" t="s">
+        <v>37</v>
+      </c>
+      <c r="C20" t="s">
+        <v>34</v>
+      </c>
+      <c r="D20" t="s">
+        <v>16</v>
+      </c>
+      <c r="E20" t="s">
+        <v>12</v>
+      </c>
+      <c r="F20" t="s">
+        <v>12</v>
+      </c>
+      <c r="G20" t="s">
+        <v>44</v>
+      </c>
+      <c r="H20" t="s">
+        <v>45</v>
+      </c>
+      <c r="I20" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9">
+      <c r="A21">
+        <v>16</v>
+      </c>
+      <c r="B21" t="s">
+        <v>37</v>
+      </c>
+      <c r="C21" t="s">
+        <v>34</v>
+      </c>
+      <c r="D21" t="s">
+        <v>16</v>
+      </c>
+      <c r="E21" t="s">
+        <v>12</v>
+      </c>
+      <c r="F21" t="s">
+        <v>12</v>
+      </c>
+      <c r="G21" t="s">
+        <v>42</v>
+      </c>
+      <c r="H21" t="s">
+        <v>43</v>
+      </c>
+      <c r="I21" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9">
+      <c r="A22">
+        <v>17</v>
+      </c>
+      <c r="B22" t="s">
+        <v>37</v>
+      </c>
+      <c r="C22" t="s">
+        <v>16</v>
+      </c>
+      <c r="D22" t="s">
+        <v>12</v>
+      </c>
+      <c r="E22" t="s">
+        <v>12</v>
+      </c>
+      <c r="F22" t="s">
+        <v>12</v>
+      </c>
+      <c r="G22" t="s">
+        <v>46</v>
+      </c>
+      <c r="H22" t="s">
+        <v>33</v>
+      </c>
+      <c r="I22" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9">
+      <c r="A23">
+        <v>18</v>
+      </c>
+      <c r="B23" t="s">
+        <v>37</v>
+      </c>
+      <c r="C23" t="s">
+        <v>16</v>
+      </c>
+      <c r="D23" t="s">
+        <v>47</v>
+      </c>
+      <c r="E23" t="s">
+        <v>12</v>
+      </c>
+      <c r="F23" t="s">
+        <v>12</v>
+      </c>
+      <c r="G23" t="s">
+        <v>48</v>
+      </c>
+      <c r="H23" t="s">
+        <v>49</v>
+      </c>
+      <c r="I23" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9">
+      <c r="A24">
+        <v>19</v>
+      </c>
+      <c r="B24" t="s">
+        <v>34</v>
+      </c>
+      <c r="C24" t="s">
+        <v>37</v>
+      </c>
+      <c r="D24" t="s">
+        <v>47</v>
+      </c>
+      <c r="E24" t="s">
+        <v>12</v>
+      </c>
+      <c r="F24" t="s">
+        <v>12</v>
+      </c>
+      <c r="G24" t="s">
+        <v>50</v>
+      </c>
+      <c r="H24" t="s">
+        <v>51</v>
+      </c>
+      <c r="I24" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9">
+      <c r="A25">
+        <v>20</v>
+      </c>
+      <c r="B25" t="s">
+        <v>34</v>
+      </c>
+      <c r="C25" t="s">
+        <v>37</v>
+      </c>
+      <c r="D25" t="s">
+        <v>47</v>
+      </c>
+      <c r="E25" t="s">
+        <v>12</v>
+      </c>
+      <c r="F25" t="s">
+        <v>12</v>
+      </c>
+      <c r="G25" t="s">
+        <v>52</v>
+      </c>
+      <c r="H25" t="s">
+        <v>53</v>
+      </c>
+      <c r="I25" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9">
+      <c r="A26">
+        <v>21</v>
+      </c>
+      <c r="B26" t="s">
+        <v>34</v>
+      </c>
+      <c r="C26" t="s">
+        <v>37</v>
+      </c>
+      <c r="D26" t="s">
+        <v>47</v>
+      </c>
+      <c r="E26" t="s">
+        <v>12</v>
+      </c>
+      <c r="F26" t="s">
+        <v>12</v>
+      </c>
+      <c r="G26" t="s">
+        <v>50</v>
+      </c>
+      <c r="H26" t="s">
+        <v>51</v>
+      </c>
+      <c r="I26" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9">
+      <c r="A27">
+        <v>22</v>
+      </c>
+      <c r="B27" t="s">
+        <v>34</v>
+      </c>
+      <c r="C27" t="s">
+        <v>47</v>
+      </c>
+      <c r="D27" t="s">
+        <v>12</v>
+      </c>
+      <c r="E27" t="s">
+        <v>12</v>
+      </c>
+      <c r="F27" t="s">
+        <v>12</v>
+      </c>
+      <c r="G27" t="s">
+        <v>54</v>
+      </c>
+      <c r="H27" t="s">
+        <v>49</v>
+      </c>
+      <c r="I27" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9">
+      <c r="A28">
+        <v>23</v>
+      </c>
+      <c r="B28" t="s">
+        <v>34</v>
+      </c>
+      <c r="C28" t="s">
+        <v>37</v>
+      </c>
+      <c r="D28" t="s">
+        <v>12</v>
+      </c>
+      <c r="E28" t="s">
+        <v>12</v>
+      </c>
+      <c r="F28" t="s">
+        <v>12</v>
+      </c>
+      <c r="G28" t="s">
+        <v>55</v>
+      </c>
+      <c r="H28" t="s">
+        <v>56</v>
+      </c>
+      <c r="I28" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9">
+      <c r="A29">
+        <v>24</v>
+      </c>
+      <c r="B29" t="s">
+        <v>34</v>
+      </c>
+      <c r="C29" t="s">
+        <v>37</v>
+      </c>
+      <c r="D29" t="s">
+        <v>12</v>
+      </c>
+      <c r="E29" t="s">
+        <v>12</v>
+      </c>
+      <c r="F29" t="s">
+        <v>12</v>
+      </c>
+      <c r="G29" t="s">
+        <v>55</v>
+      </c>
+      <c r="H29" t="s">
+        <v>57</v>
+      </c>
+      <c r="I29" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9">
+      <c r="A30">
+        <v>25</v>
+      </c>
+      <c r="B30" t="s">
+        <v>34</v>
+      </c>
+      <c r="C30" t="s">
+        <v>37</v>
+      </c>
+      <c r="D30" t="s">
+        <v>12</v>
+      </c>
+      <c r="E30" t="s">
+        <v>12</v>
+      </c>
+      <c r="F30" t="s">
+        <v>12</v>
+      </c>
+      <c r="G30" t="s">
+        <v>55</v>
+      </c>
+      <c r="H30" t="s">
+        <v>56</v>
+      </c>
+      <c r="I30" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9">
+      <c r="A31">
+        <v>26</v>
+      </c>
+      <c r="B31" t="s">
+        <v>37</v>
+      </c>
+      <c r="C31" t="s">
+        <v>12</v>
+      </c>
+      <c r="D31" t="s">
+        <v>12</v>
+      </c>
+      <c r="E31" t="s">
+        <v>12</v>
+      </c>
+      <c r="F31" t="s">
+        <v>12</v>
+      </c>
+      <c r="G31" t="s">
+        <v>58</v>
+      </c>
+      <c r="H31" t="s">
+        <v>49</v>
+      </c>
+      <c r="I31" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9">
+      <c r="A32">
+        <v>27</v>
+      </c>
+      <c r="B32" t="s">
+        <v>37</v>
+      </c>
+      <c r="C32" t="s">
+        <v>59</v>
+      </c>
+      <c r="D32" t="s">
+        <v>12</v>
+      </c>
+      <c r="E32" t="s">
+        <v>12</v>
+      </c>
+      <c r="F32" t="s">
+        <v>12</v>
+      </c>
+      <c r="G32" t="s">
+        <v>60</v>
+      </c>
+      <c r="H32" t="s">
+        <v>61</v>
+      </c>
+      <c r="I32" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9">
+      <c r="A33">
+        <v>28</v>
+      </c>
+      <c r="B33" t="s">
+        <v>34</v>
+      </c>
+      <c r="C33" t="s">
+        <v>59</v>
+      </c>
+      <c r="D33" t="s">
+        <v>12</v>
+      </c>
+      <c r="E33" t="s">
+        <v>12</v>
+      </c>
+      <c r="F33" t="s">
+        <v>12</v>
+      </c>
+      <c r="G33" t="s">
+        <v>62</v>
+      </c>
+      <c r="H33" t="s">
+        <v>63</v>
+      </c>
+      <c r="I33" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9">
+      <c r="A34">
+        <v>29</v>
+      </c>
+      <c r="B34" t="s">
+        <v>37</v>
+      </c>
+      <c r="C34" t="s">
+        <v>34</v>
+      </c>
+      <c r="D34" t="s">
+        <v>59</v>
+      </c>
+      <c r="E34" t="s">
+        <v>12</v>
+      </c>
+      <c r="F34" t="s">
+        <v>12</v>
+      </c>
+      <c r="G34" t="s">
+        <v>64</v>
+      </c>
+      <c r="H34" t="s">
+        <v>65</v>
+      </c>
+      <c r="I34" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9">
+      <c r="A35">
         <v>30</v>
       </c>
-      <c r="C20" t="s">
-        <v>18</v>
-      </c>
-      <c r="D20" t="s">
-        <v>12</v>
-      </c>
-      <c r="E20" t="s">
-        <v>12</v>
-      </c>
-      <c r="F20" t="s">
-        <v>12</v>
-      </c>
-      <c r="G20" t="s">
+      <c r="B35" t="s">
+        <v>37</v>
+      </c>
+      <c r="C35" t="s">
+        <v>34</v>
+      </c>
+      <c r="D35" t="s">
+        <v>59</v>
+      </c>
+      <c r="E35" t="s">
+        <v>12</v>
+      </c>
+      <c r="F35" t="s">
+        <v>12</v>
+      </c>
+      <c r="G35" t="s">
+        <v>66</v>
+      </c>
+      <c r="H35" t="s">
+        <v>63</v>
+      </c>
+      <c r="I35" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9">
+      <c r="A36">
         <v>31</v>
       </c>
-      <c r="H20" t="s">
-        <v>14</v>
-      </c>
-      <c r="I20" s="3" t="s">
-        <v>15</v>
+      <c r="B36" t="s">
+        <v>34</v>
+      </c>
+      <c r="C36" t="s">
+        <v>59</v>
+      </c>
+      <c r="D36" t="s">
+        <v>12</v>
+      </c>
+      <c r="E36" t="s">
+        <v>12</v>
+      </c>
+      <c r="F36" t="s">
+        <v>12</v>
+      </c>
+      <c r="G36" t="s">
+        <v>67</v>
+      </c>
+      <c r="H36" t="s">
+        <v>61</v>
+      </c>
+      <c r="I36" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9">
+      <c r="A37">
+        <v>32</v>
+      </c>
+      <c r="B37" t="s">
+        <v>37</v>
+      </c>
+      <c r="C37" t="s">
+        <v>59</v>
+      </c>
+      <c r="D37" t="s">
+        <v>12</v>
+      </c>
+      <c r="E37" t="s">
+        <v>12</v>
+      </c>
+      <c r="F37" t="s">
+        <v>12</v>
+      </c>
+      <c r="G37" t="s">
+        <v>68</v>
+      </c>
+      <c r="H37" t="s">
+        <v>69</v>
+      </c>
+      <c r="I37" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9">
+      <c r="A38">
+        <v>33</v>
+      </c>
+      <c r="B38" t="s">
+        <v>34</v>
+      </c>
+      <c r="C38" t="s">
+        <v>37</v>
+      </c>
+      <c r="D38" t="s">
+        <v>59</v>
+      </c>
+      <c r="E38" t="s">
+        <v>12</v>
+      </c>
+      <c r="F38" t="s">
+        <v>12</v>
+      </c>
+      <c r="G38" t="s">
+        <v>70</v>
+      </c>
+      <c r="H38" t="s">
+        <v>71</v>
+      </c>
+      <c r="I38" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9">
+      <c r="A39">
+        <v>34</v>
+      </c>
+      <c r="B39" t="s">
+        <v>34</v>
+      </c>
+      <c r="C39" t="s">
+        <v>37</v>
+      </c>
+      <c r="D39" t="s">
+        <v>59</v>
+      </c>
+      <c r="E39" t="s">
+        <v>12</v>
+      </c>
+      <c r="F39" t="s">
+        <v>12</v>
+      </c>
+      <c r="G39" t="s">
+        <v>72</v>
+      </c>
+      <c r="H39" t="s">
+        <v>69</v>
+      </c>
+      <c r="I39" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9">
+      <c r="A40">
+        <v>35</v>
+      </c>
+      <c r="B40" t="s">
+        <v>37</v>
+      </c>
+      <c r="C40" t="s">
+        <v>59</v>
+      </c>
+      <c r="D40" t="s">
+        <v>12</v>
+      </c>
+      <c r="E40" t="s">
+        <v>12</v>
+      </c>
+      <c r="F40" t="s">
+        <v>12</v>
+      </c>
+      <c r="G40" t="s">
+        <v>60</v>
+      </c>
+      <c r="H40" t="s">
+        <v>61</v>
+      </c>
+      <c r="I40" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9">
+      <c r="A41">
+        <v>36</v>
+      </c>
+      <c r="B41" t="s">
+        <v>37</v>
+      </c>
+      <c r="C41" t="s">
+        <v>73</v>
+      </c>
+      <c r="D41" t="s">
+        <v>12</v>
+      </c>
+      <c r="E41" t="s">
+        <v>12</v>
+      </c>
+      <c r="F41" t="s">
+        <v>12</v>
+      </c>
+      <c r="G41" t="s">
+        <v>74</v>
+      </c>
+      <c r="H41" t="s">
+        <v>75</v>
+      </c>
+      <c r="I41" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9">
+      <c r="A42">
+        <v>37</v>
+      </c>
+      <c r="B42" t="s">
+        <v>34</v>
+      </c>
+      <c r="C42" t="s">
+        <v>73</v>
+      </c>
+      <c r="D42" t="s">
+        <v>12</v>
+      </c>
+      <c r="E42" t="s">
+        <v>12</v>
+      </c>
+      <c r="F42" t="s">
+        <v>12</v>
+      </c>
+      <c r="G42" t="s">
+        <v>76</v>
+      </c>
+      <c r="H42" t="s">
+        <v>77</v>
+      </c>
+      <c r="I42" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9">
+      <c r="A43">
+        <v>38</v>
+      </c>
+      <c r="B43" t="s">
+        <v>37</v>
+      </c>
+      <c r="C43" t="s">
+        <v>34</v>
+      </c>
+      <c r="D43" t="s">
+        <v>73</v>
+      </c>
+      <c r="E43" t="s">
+        <v>12</v>
+      </c>
+      <c r="F43" t="s">
+        <v>12</v>
+      </c>
+      <c r="G43" t="s">
+        <v>78</v>
+      </c>
+      <c r="H43" t="s">
+        <v>79</v>
+      </c>
+      <c r="I43" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9">
+      <c r="A44">
+        <v>39</v>
+      </c>
+      <c r="B44" t="s">
+        <v>37</v>
+      </c>
+      <c r="C44" t="s">
+        <v>34</v>
+      </c>
+      <c r="D44" t="s">
+        <v>73</v>
+      </c>
+      <c r="E44" t="s">
+        <v>12</v>
+      </c>
+      <c r="F44" t="s">
+        <v>12</v>
+      </c>
+      <c r="G44" t="s">
+        <v>80</v>
+      </c>
+      <c r="H44" t="s">
+        <v>77</v>
+      </c>
+      <c r="I44" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9">
+      <c r="A45">
+        <v>40</v>
+      </c>
+      <c r="B45" t="s">
+        <v>34</v>
+      </c>
+      <c r="C45" t="s">
+        <v>73</v>
+      </c>
+      <c r="D45" t="s">
+        <v>12</v>
+      </c>
+      <c r="E45" t="s">
+        <v>12</v>
+      </c>
+      <c r="F45" t="s">
+        <v>12</v>
+      </c>
+      <c r="G45" t="s">
+        <v>81</v>
+      </c>
+      <c r="H45" t="s">
+        <v>75</v>
+      </c>
+      <c r="I45" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9">
+      <c r="A46">
+        <v>41</v>
+      </c>
+      <c r="B46" t="s">
+        <v>37</v>
+      </c>
+      <c r="C46" t="s">
+        <v>73</v>
+      </c>
+      <c r="D46" t="s">
+        <v>12</v>
+      </c>
+      <c r="E46" t="s">
+        <v>12</v>
+      </c>
+      <c r="F46" t="s">
+        <v>12</v>
+      </c>
+      <c r="G46" t="s">
+        <v>82</v>
+      </c>
+      <c r="H46" t="s">
+        <v>83</v>
+      </c>
+      <c r="I46" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9">
+      <c r="A47">
+        <v>42</v>
+      </c>
+      <c r="B47" t="s">
+        <v>34</v>
+      </c>
+      <c r="C47" t="s">
+        <v>37</v>
+      </c>
+      <c r="D47" t="s">
+        <v>73</v>
+      </c>
+      <c r="E47" t="s">
+        <v>12</v>
+      </c>
+      <c r="F47" t="s">
+        <v>12</v>
+      </c>
+      <c r="G47" t="s">
+        <v>84</v>
+      </c>
+      <c r="H47" t="s">
+        <v>85</v>
+      </c>
+      <c r="I47" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9">
+      <c r="A48">
+        <v>43</v>
+      </c>
+      <c r="B48" t="s">
+        <v>34</v>
+      </c>
+      <c r="C48" t="s">
+        <v>37</v>
+      </c>
+      <c r="D48" t="s">
+        <v>73</v>
+      </c>
+      <c r="E48" t="s">
+        <v>12</v>
+      </c>
+      <c r="F48" t="s">
+        <v>12</v>
+      </c>
+      <c r="G48" t="s">
+        <v>86</v>
+      </c>
+      <c r="H48" t="s">
+        <v>83</v>
+      </c>
+      <c r="I48" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9">
+      <c r="A49">
+        <v>44</v>
+      </c>
+      <c r="B49" t="s">
+        <v>37</v>
+      </c>
+      <c r="C49" t="s">
+        <v>73</v>
+      </c>
+      <c r="D49" t="s">
+        <v>12</v>
+      </c>
+      <c r="E49" t="s">
+        <v>12</v>
+      </c>
+      <c r="F49" t="s">
+        <v>12</v>
+      </c>
+      <c r="G49" t="s">
+        <v>74</v>
+      </c>
+      <c r="H49" t="s">
+        <v>75</v>
+      </c>
+      <c r="I49" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9">
+      <c r="A50">
+        <v>45</v>
+      </c>
+      <c r="B50" t="s">
+        <v>37</v>
+      </c>
+      <c r="C50" t="s">
+        <v>19</v>
+      </c>
+      <c r="D50" t="s">
+        <v>73</v>
+      </c>
+      <c r="E50" t="s">
+        <v>12</v>
+      </c>
+      <c r="F50" t="s">
+        <v>12</v>
+      </c>
+      <c r="G50" t="s">
+        <v>87</v>
+      </c>
+      <c r="H50" t="s">
+        <v>19</v>
+      </c>
+      <c r="I50" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9">
+      <c r="A51">
+        <v>46</v>
+      </c>
+      <c r="B51" t="s">
+        <v>37</v>
+      </c>
+      <c r="C51" t="s">
+        <v>19</v>
+      </c>
+      <c r="D51" t="s">
+        <v>31</v>
+      </c>
+      <c r="E51" t="s">
+        <v>12</v>
+      </c>
+      <c r="F51" t="s">
+        <v>12</v>
+      </c>
+      <c r="G51" t="s">
+        <v>88</v>
+      </c>
+      <c r="H51" t="s">
+        <v>89</v>
+      </c>
+      <c r="I51" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9">
+      <c r="A52">
+        <v>47</v>
+      </c>
+      <c r="B52" t="s">
+        <v>34</v>
+      </c>
+      <c r="C52" t="s">
+        <v>19</v>
+      </c>
+      <c r="D52" t="s">
+        <v>31</v>
+      </c>
+      <c r="E52" t="s">
+        <v>12</v>
+      </c>
+      <c r="F52" t="s">
+        <v>12</v>
+      </c>
+      <c r="G52" t="s">
+        <v>90</v>
+      </c>
+      <c r="H52" t="s">
+        <v>91</v>
+      </c>
+      <c r="I52" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9">
+      <c r="A53">
+        <v>48</v>
+      </c>
+      <c r="B53" t="s">
+        <v>37</v>
+      </c>
+      <c r="C53" t="s">
+        <v>34</v>
+      </c>
+      <c r="D53" t="s">
+        <v>19</v>
+      </c>
+      <c r="E53" t="s">
+        <v>31</v>
+      </c>
+      <c r="F53" t="s">
+        <v>12</v>
+      </c>
+      <c r="G53" t="s">
+        <v>92</v>
+      </c>
+      <c r="H53" t="s">
+        <v>93</v>
+      </c>
+      <c r="I53" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9">
+      <c r="A54">
+        <v>49</v>
+      </c>
+      <c r="B54" t="s">
+        <v>37</v>
+      </c>
+      <c r="C54" t="s">
+        <v>34</v>
+      </c>
+      <c r="D54" t="s">
+        <v>19</v>
+      </c>
+      <c r="E54" t="s">
+        <v>31</v>
+      </c>
+      <c r="F54" t="s">
+        <v>12</v>
+      </c>
+      <c r="G54" t="s">
+        <v>92</v>
+      </c>
+      <c r="H54" t="s">
+        <v>91</v>
+      </c>
+      <c r="I54" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9">
+      <c r="A55">
+        <v>50</v>
+      </c>
+      <c r="B55" t="s">
+        <v>34</v>
+      </c>
+      <c r="C55" t="s">
+        <v>19</v>
+      </c>
+      <c r="D55" t="s">
+        <v>31</v>
+      </c>
+      <c r="E55" t="s">
+        <v>12</v>
+      </c>
+      <c r="F55" t="s">
+        <v>12</v>
+      </c>
+      <c r="G55" t="s">
+        <v>94</v>
+      </c>
+      <c r="H55" t="s">
+        <v>89</v>
+      </c>
+      <c r="I55" s="5" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>